<commit_message>
add gfed fire emissions
</commit_message>
<xml_diff>
--- a/results/section_2_2_table_2024.xlsx
+++ b/results/section_2_2_table_2024.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t xml:space="preserve">label</t>
   </si>
@@ -32,13 +32,10 @@
     <t xml:space="preserve">2010-2019</t>
   </si>
   <si>
-    <t xml:space="preserve">2012-2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 (projection)</t>
+    <t xml:space="preserve">2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 (projection)</t>
   </si>
   <si>
     <t xml:space="preserve">GHG</t>
@@ -53,13 +50,13 @@
     <t xml:space="preserve">39±5.1</t>
   </si>
   <si>
-    <t xml:space="preserve">45±5.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">53±5.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">55±5.3</t>
+    <t xml:space="preserve">46±5.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">53±5.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55±5.4</t>
   </si>
   <si>
     <t xml:space="preserve">CO2-FFI</t>
@@ -80,15 +77,12 @@
     <t xml:space="preserve">35±2.8</t>
   </si>
   <si>
-    <t xml:space="preserve">36±2.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37±2.9</t>
-  </si>
-  <si>
     <t xml:space="preserve">37±3</t>
   </si>
   <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
     <t xml:space="preserve">CO2-LULUCF</t>
   </si>
   <si>
@@ -107,15 +101,9 @@
     <t xml:space="preserve">5±3.5</t>
   </si>
   <si>
-    <t xml:space="preserve">4.8±3.3</t>
-  </si>
-  <si>
     <t xml:space="preserve">4.3±3</t>
   </si>
   <si>
-    <t xml:space="preserve">3.9±2.8</t>
-  </si>
-  <si>
     <t xml:space="preserve">CH4</t>
   </si>
   <si>
@@ -125,16 +113,16 @@
     <t xml:space="preserve">6.5±2</t>
   </si>
   <si>
-    <t xml:space="preserve">7±2.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.7±2.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.4±2.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.6±2.6</t>
+    <t xml:space="preserve">7.2±2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.1±2.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.8±2.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9±2.7</t>
   </si>
   <si>
     <t xml:space="preserve">N2O</t>
@@ -146,43 +134,37 @@
     <t xml:space="preserve">2.1±1.2</t>
   </si>
   <si>
-    <t xml:space="preserve">2.2±1.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.4±1.5</t>
+    <t xml:space="preserve">2.3±1.4</t>
   </si>
   <si>
     <t xml:space="preserve">2.7±1.6</t>
   </si>
   <si>
-    <t xml:space="preserve">2.8±1.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.9±1.7</t>
+    <t xml:space="preserve">2.9±1.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.1±1.9</t>
   </si>
   <si>
     <t xml:space="preserve">F-gases</t>
   </si>
   <si>
-    <t xml:space="preserve">0.58±0.17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.78±0.23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.77±0.23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1±0.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.5±0.46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.7±0.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2±0.59</t>
+    <t xml:space="preserve">0.53±0.16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.64±0.19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.55±0.16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.74±0.22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1±0.34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.4±0.43</t>
   </si>
 </sst>
 </file>
@@ -539,175 +521,154 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2"/>
+      <c r="H2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>20</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>21</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>26</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>27</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>28</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>29</v>
       </c>
-      <c r="F4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" t="s">
-        <v>31</v>
-      </c>
       <c r="H4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
         <v>34</v>
       </c>
-      <c r="B5" t="s">
+      <c r="F5" t="s">
         <v>35</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G5" t="s">
         <v>36</v>
       </c>
-      <c r="D5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5"/>
+      <c r="H5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" t="s">
         <v>41</v>
       </c>
-      <c r="B6" t="s">
+      <c r="F6" t="s">
         <v>42</v>
       </c>
-      <c r="C6" t="s">
+      <c r="G6" t="s">
         <v>43</v>
       </c>
-      <c r="D6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" t="s">
-        <v>47</v>
-      </c>
-      <c r="H6" t="s">
-        <v>48</v>
-      </c>
-      <c r="I6"/>
+      <c r="H6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" t="s">
         <v>49</v>
       </c>
-      <c r="B7" t="s">
+      <c r="G7" t="s">
         <v>50</v>
       </c>
-      <c r="C7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H7" t="s">
-        <v>56</v>
-      </c>
-      <c r="I7"/>
+      <c r="H7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>